<commit_message>
Modifier analyse monte carlo
</commit_message>
<xml_diff>
--- a/HiRelRapport_CourantTension_Maret_Gsponer/WCA/result.xlsx
+++ b/HiRelRapport_CourantTension_Maret_Gsponer/WCA/result.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emilie\Documents\Git Hub\HiRel\MonteCarlo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emilie\Documents\Git Hub\HiRel\HiRelRapport_CourantTension_Maret_Gsponer\WCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="4" sheetId="4" r:id="rId1"/>
-    <sheet name="Diagram 5" sheetId="3" r:id="rId2"/>
-    <sheet name="5" sheetId="2" r:id="rId3"/>
-    <sheet name="Feuil1" sheetId="1" r:id="rId4"/>
+    <sheet name="Diagram 1" sheetId="9" r:id="rId1"/>
+    <sheet name="1" sheetId="8" r:id="rId2"/>
+    <sheet name="Diagram 2" sheetId="7" r:id="rId3"/>
+    <sheet name="2" sheetId="6" r:id="rId4"/>
+    <sheet name="Diagram 3" sheetId="5" r:id="rId5"/>
+    <sheet name="3" sheetId="4" r:id="rId6"/>
+    <sheet name="Diagram 4" sheetId="3" r:id="rId7"/>
+    <sheet name="4" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -103,325 +107,325 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'5'!$A$1:$A$50</c:f>
+              <c:f>'1'!$A$1:$A$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>3.8862904127590161</c:v>
+                  <c:v>9.9000094459101573E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8908439611286609</c:v>
+                  <c:v>9.904013048555213E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8953975094983053</c:v>
+                  <c:v>9.9080166512002674E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8999510578679502</c:v>
+                  <c:v>9.9120202538453217E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.904504606237595</c:v>
+                  <c:v>9.9160238564903774E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9090581546072394</c:v>
+                  <c:v>9.9200274591354332E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.9136117029768842</c:v>
+                  <c:v>9.9240310617804875E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.918165251346529</c:v>
+                  <c:v>9.9280346644255418E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.9227187997161734</c:v>
+                  <c:v>9.9320382670705976E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9272723480858183</c:v>
+                  <c:v>9.9360418697156533E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.9318258964554631</c:v>
+                  <c:v>9.9400454723607076E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9363794448251075</c:v>
+                  <c:v>9.944049075005762E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9409329931947523</c:v>
+                  <c:v>9.9480526776508177E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.9454865415643972</c:v>
+                  <c:v>9.9520562802958734E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.950040089934042</c:v>
+                  <c:v>9.9560598829409278E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.9545936383036864</c:v>
+                  <c:v>9.9600634855859821E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.9591471866733312</c:v>
+                  <c:v>9.9640670882310378E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.963700735042976</c:v>
+                  <c:v>9.9680706908760935E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.9682542834126204</c:v>
+                  <c:v>9.9720742935211479E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.9728078317822653</c:v>
+                  <c:v>9.9760778961662022E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.9773613801519101</c:v>
+                  <c:v>9.9800814988112579E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.9819149285215545</c:v>
+                  <c:v>9.9840851014563137E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.9864684768911993</c:v>
+                  <c:v>9.988088704101368E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.9910220252608442</c:v>
+                  <c:v>9.9920923067464223E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.9955755736304885</c:v>
+                  <c:v>9.9960959093914781E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.0001291220001338</c:v>
+                  <c:v>0.10000099512036534</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.0046826703697782</c:v>
+                  <c:v>0.10004103114681588</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0092362187394226</c:v>
+                  <c:v>0.10008106717326642</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.013789767109067</c:v>
+                  <c:v>0.10012110319971698</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.0183433154787123</c:v>
+                  <c:v>0.10016113922616754</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.0228968638483567</c:v>
+                  <c:v>0.10020117525261808</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.0274504122180019</c:v>
+                  <c:v>0.10024121127906863</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.0320039605876463</c:v>
+                  <c:v>0.10028124730551918</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.0365575089572907</c:v>
+                  <c:v>0.10032128333196974</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.041111057326936</c:v>
+                  <c:v>0.10036131935842028</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.0456646056965804</c:v>
+                  <c:v>0.10040135538487083</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.0502181540662248</c:v>
+                  <c:v>0.10044139141132138</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.05477170243587</c:v>
+                  <c:v>0.10048142743777194</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.0593252508055144</c:v>
+                  <c:v>0.10052146346422249</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.0638787991751588</c:v>
+                  <c:v>0.10056149949067303</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.0684323475448041</c:v>
+                  <c:v>0.10060153551712359</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.0729858959144485</c:v>
+                  <c:v>0.10064157154357414</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.0775394442840929</c:v>
+                  <c:v>0.10068160757002469</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.0820929926537382</c:v>
+                  <c:v>0.10072164359647523</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.0866465410233825</c:v>
+                  <c:v>0.10076167962292579</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.0912000893930269</c:v>
+                  <c:v>0.10080171564937634</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.0957536377626722</c:v>
+                  <c:v>0.10084175167582689</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.1003071861323166</c:v>
+                  <c:v>0.10088178770227743</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.104860734501961</c:v>
+                  <c:v>0.10092182372872799</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.1094142828716063</c:v>
+                  <c:v>0.10096185975517855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'5'!$B$1:$B$50</c:f>
+              <c:f>'1'!$B$1:$B$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>27</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43</c:v>
+                  <c:v>199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>77</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97</c:v>
+                  <c:v>226</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>111</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>123</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>152</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>199</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>182</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>236</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>265</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>318</c:v>
+                  <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>318</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>337</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>343</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>360</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>421</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>392</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>432</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>439</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>395</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>450</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>421</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>402</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>407</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>365</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>344</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>372</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>268</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>264</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>215</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>195</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>176</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>163</c:v>
+                  <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>111</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>113</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>98</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>66</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>68</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>35</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>30</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>24</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>22</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>9</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6</c:v>
+                  <c:v>159</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AF88-46DA-B945-03D0DAA4E341}"/>
+              <c16:uniqueId val="{00000000-C75C-4B47-A409-A61CE07677A0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -434,11 +438,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="462151272"/>
-        <c:axId val="462149632"/>
+        <c:axId val="329726864"/>
+        <c:axId val="329728176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="462151272"/>
+        <c:axId val="329726864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -448,7 +452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="462149632"/>
+        <c:crossAx val="329728176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -456,7 +460,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="462149632"/>
+        <c:axId val="329728176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +471,1228 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="462151272"/>
+        <c:crossAx val="329726864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2'!$A$1:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>99.000128006273357</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.040154964421902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>99.080181922570432</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.120208880718977</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99.160235838867521</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.200262797016052</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>99.240289755164596</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>99.280316713313141</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>99.320343671461671</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.360370629610216</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>99.400397587758761</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>99.440424545907291</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>99.480451504055836</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99.52047846220438</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>99.560505420352911</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>99.600532378501455</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>99.64055933665</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>99.68058629479853</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99.720613252947075</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99.76064021109562</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>99.80066716924415</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>99.840694127392695</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99.880721085541239</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>99.92074804368977</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>99.960775001838314</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>100.00080195998686</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>100.04082891813539</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>100.08085587628393</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>100.12088283443246</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>100.16090979258101</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>100.20093675072955</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>100.24096370887808</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>100.28099066702663</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>100.32101762517517</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>100.3610445833237</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>100.40107154147225</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100.44109849962079</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>100.48112545776932</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>100.52115241591787</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>100.56117937406641</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>100.60120633221494</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>100.64123329036349</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>100.68126024851203</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>100.72128720666056</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100.76131416480911</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>100.80134112295765</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>100.84136808110618</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>100.88139503925473</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>100.92142199740327</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>100.9614489555518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2'!$B$1:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>193</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>198</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EECD-4894-A82E-85B6C25F8141}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:axId val="327982440"/>
+        <c:axId val="327979816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="327982440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="327979816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="327979816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="327982440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'3'!$A$1:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>19800.069861439828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19808.07616823824</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19816.082475036648</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19824.08878183506</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19832.095088633469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19840.101395431881</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19848.107702230289</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19856.114009028701</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19864.120315827109</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19872.126622625521</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19880.132929423929</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19888.139236222341</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19896.14554302075</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19904.151849819162</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19912.15815661757</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19920.164463415982</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19928.17077021439</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19936.177077012802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19944.183383811211</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19952.189690609623</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19960.195997408031</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19968.202304206443</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19976.208611004851</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19984.214917803263</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19992.221224601672</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20000.227531400084</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20008.233838198496</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20016.240144996904</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20024.246451795316</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20032.252758593724</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20040.259065392136</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20048.265372190544</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20056.271678988956</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20064.277985787365</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20072.284292585777</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20080.290599384185</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20088.296906182597</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20096.303212981005</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20104.309519779417</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20112.315826577826</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20120.322133376238</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20128.328440174646</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20136.334746973058</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20144.341053771466</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20152.347360569878</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20160.353667368287</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20168.359974166699</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20176.366280965107</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20184.372587763519</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20192.378894561927</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3'!$B$1:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>204</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>203</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>205</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>198</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>208</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DF3C-49F4-9A2A-79356CB3DF6D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:axId val="327980472"/>
+        <c:axId val="327979160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="327980472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="327979160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="327979160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="327980472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'4'!$A$1:$A$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>19.430968263251035</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.453834612667048</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.476700962083061</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.499567311499074</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.522433660915087</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.545300010331104</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.568166359747117</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.59103270916313</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.613899058579143</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19.636765407995156</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.659631757411169</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.682498106827182</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.705364456243196</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.728230805659209</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.751097155075222</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.773963504491235</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.796829853907251</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.819696203323264</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.842562552739277</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.865428902155291</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19.888295251571304</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19.911161600987317</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19.93402795040333</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19.956894299819343</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>19.979760649235356</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20.002626998651373</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20.025493348067386</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20.048359697483399</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20.071226046899412</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20.094092396315425</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20.116958745731438</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>20.139825095147451</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20.162691444563464</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>20.185557793979477</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.20842414339549</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20.231290492811503</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>20.25415684222752</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>20.277023191643533</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20.299889541059546</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>20.322755890475559</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20.345622239891572</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20.368488589307585</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20.391354938723598</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20.414221288139611</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>20.437087637555624</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20.459953986971641</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20.482820336387654</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20.505686685803667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20.52855303521968</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.551419384635693</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'4'!$B$1:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>222</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>254</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>302</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>327</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>423</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>387</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>429</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>432</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>396</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>417</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>274</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>232</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD4A-4B6E-9E14-1D003C12240E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:axId val="328723032"/>
+        <c:axId val="328722376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="328723032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="328722376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="328722376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="328723032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -487,7 +1712,40 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="84" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="84" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="84" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -498,7 +1756,88 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9292354" cy="6062283"/>
+    <xdr:ext cx="9289143" cy="6059714"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9289143" cy="6059714"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9289143" cy="6059714"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9289143" cy="6059714"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
@@ -818,12 +2157,413 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>9.9000094459101573E-2</v>
+      </c>
+      <c r="B1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>9.904013048555213E-2</v>
+      </c>
+      <c r="B2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>9.9080166512002674E-2</v>
+      </c>
+      <c r="B3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9.9120202538453217E-2</v>
+      </c>
+      <c r="B4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>9.9160238564903774E-2</v>
+      </c>
+      <c r="B5">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>9.9200274591354332E-2</v>
+      </c>
+      <c r="B6">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>9.9240310617804875E-2</v>
+      </c>
+      <c r="B7">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>9.9280346644255418E-2</v>
+      </c>
+      <c r="B8">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>9.9320382670705976E-2</v>
+      </c>
+      <c r="B9">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9.9360418697156533E-2</v>
+      </c>
+      <c r="B10">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9.9400454723607076E-2</v>
+      </c>
+      <c r="B11">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9.944049075005762E-2</v>
+      </c>
+      <c r="B12">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9.9480526776508177E-2</v>
+      </c>
+      <c r="B13">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>9.9520562802958734E-2</v>
+      </c>
+      <c r="B14">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>9.9560598829409278E-2</v>
+      </c>
+      <c r="B15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>9.9600634855859821E-2</v>
+      </c>
+      <c r="B16">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>9.9640670882310378E-2</v>
+      </c>
+      <c r="B17">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>9.9680706908760935E-2</v>
+      </c>
+      <c r="B18">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>9.9720742935211479E-2</v>
+      </c>
+      <c r="B19">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>9.9760778961662022E-2</v>
+      </c>
+      <c r="B20">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>9.9800814988112579E-2</v>
+      </c>
+      <c r="B21">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>9.9840851014563137E-2</v>
+      </c>
+      <c r="B22">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>9.988088704101368E-2</v>
+      </c>
+      <c r="B23">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>9.9920923067464223E-2</v>
+      </c>
+      <c r="B24">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>9.9960959093914781E-2</v>
+      </c>
+      <c r="B25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0.10000099512036534</v>
+      </c>
+      <c r="B26">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.10004103114681588</v>
+      </c>
+      <c r="B27">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.10008106717326642</v>
+      </c>
+      <c r="B28">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0.10012110319971698</v>
+      </c>
+      <c r="B29">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.10016113922616754</v>
+      </c>
+      <c r="B30">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0.10020117525261808</v>
+      </c>
+      <c r="B31">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.10024121127906863</v>
+      </c>
+      <c r="B32">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0.10028124730551918</v>
+      </c>
+      <c r="B33">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0.10032128333196974</v>
+      </c>
+      <c r="B34">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0.10036131935842028</v>
+      </c>
+      <c r="B35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0.10040135538487083</v>
+      </c>
+      <c r="B36">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0.10044139141132138</v>
+      </c>
+      <c r="B37">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0.10048142743777194</v>
+      </c>
+      <c r="B38">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0.10052146346422249</v>
+      </c>
+      <c r="B39">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0.10056149949067303</v>
+      </c>
+      <c r="B40">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0.10060153551712359</v>
+      </c>
+      <c r="B41">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0.10064157154357414</v>
+      </c>
+      <c r="B42">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0.10068160757002469</v>
+      </c>
+      <c r="B43">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0.10072164359647523</v>
+      </c>
+      <c r="B44">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0.10076167962292579</v>
+      </c>
+      <c r="B45">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0.10080171564937634</v>
+      </c>
+      <c r="B46">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0.10084175167582689</v>
+      </c>
+      <c r="B47">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0.10088178770227743</v>
+      </c>
+      <c r="B48">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0.10092182372872799</v>
+      </c>
+      <c r="B49">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0.10096185975517855</v>
+      </c>
+      <c r="B50">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -838,402 +2578,402 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>3.8862904127590161</v>
+        <v>99.000128006273357</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3.8908439611286609</v>
+        <v>99.040154964421902</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>3.8953975094983053</v>
+        <v>99.080181922570432</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3.8999510578679502</v>
+        <v>99.120208880718977</v>
       </c>
       <c r="B4">
-        <v>27</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3.904504606237595</v>
+        <v>99.160235838867521</v>
       </c>
       <c r="B5">
-        <v>27</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3.9090581546072394</v>
+        <v>99.200262797016052</v>
       </c>
       <c r="B6">
-        <v>43</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3.9136117029768842</v>
+        <v>99.240289755164596</v>
       </c>
       <c r="B7">
-        <v>57</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3.918165251346529</v>
+        <v>99.280316713313141</v>
       </c>
       <c r="B8">
-        <v>77</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3.9227187997161734</v>
+        <v>99.320343671461671</v>
       </c>
       <c r="B9">
-        <v>97</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>3.9272723480858183</v>
+        <v>99.360370629610216</v>
       </c>
       <c r="B10">
-        <v>111</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>3.9318258964554631</v>
+        <v>99.400397587758761</v>
       </c>
       <c r="B11">
-        <v>123</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3.9363794448251075</v>
+        <v>99.440424545907291</v>
       </c>
       <c r="B12">
-        <v>152</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3.9409329931947523</v>
+        <v>99.480451504055836</v>
       </c>
       <c r="B13">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3.9454865415643972</v>
+        <v>99.52047846220438</v>
       </c>
       <c r="B14">
-        <v>182</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3.950040089934042</v>
+        <v>99.560505420352911</v>
       </c>
       <c r="B15">
-        <v>236</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3.9545936383036864</v>
+        <v>99.600532378501455</v>
       </c>
       <c r="B16">
-        <v>265</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>3.9591471866733312</v>
+        <v>99.64055933665</v>
       </c>
       <c r="B17">
-        <v>318</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>3.963700735042976</v>
+        <v>99.68058629479853</v>
       </c>
       <c r="B18">
-        <v>318</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>3.9682542834126204</v>
+        <v>99.720613252947075</v>
       </c>
       <c r="B19">
-        <v>337</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>3.9728078317822653</v>
+        <v>99.76064021109562</v>
       </c>
       <c r="B20">
-        <v>343</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>3.9773613801519101</v>
+        <v>99.80066716924415</v>
       </c>
       <c r="B21">
-        <v>360</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>3.9819149285215545</v>
+        <v>99.840694127392695</v>
       </c>
       <c r="B22">
-        <v>421</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>3.9864684768911993</v>
+        <v>99.880721085541239</v>
       </c>
       <c r="B23">
-        <v>392</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>3.9910220252608442</v>
+        <v>99.92074804368977</v>
       </c>
       <c r="B24">
-        <v>432</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>3.9955755736304885</v>
+        <v>99.960775001838314</v>
       </c>
       <c r="B25">
-        <v>439</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>4.0001291220001338</v>
+        <v>100.00080195998686</v>
       </c>
       <c r="B26">
-        <v>395</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>4.0046826703697782</v>
+        <v>100.04082891813539</v>
       </c>
       <c r="B27">
-        <v>450</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>4.0092362187394226</v>
+        <v>100.08085587628393</v>
       </c>
       <c r="B28">
-        <v>421</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>4.013789767109067</v>
+        <v>100.12088283443246</v>
       </c>
       <c r="B29">
-        <v>402</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>4.0183433154787123</v>
+        <v>100.16090979258101</v>
       </c>
       <c r="B30">
-        <v>407</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>4.0228968638483567</v>
+        <v>100.20093675072955</v>
       </c>
       <c r="B31">
-        <v>365</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>4.0274504122180019</v>
+        <v>100.24096370887808</v>
       </c>
       <c r="B32">
-        <v>344</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>4.0320039605876463</v>
+        <v>100.28099066702663</v>
       </c>
       <c r="B33">
-        <v>372</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>4.0365575089572907</v>
+        <v>100.32101762517517</v>
       </c>
       <c r="B34">
-        <v>268</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>4.041111057326936</v>
+        <v>100.3610445833237</v>
       </c>
       <c r="B35">
-        <v>264</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>4.0456646056965804</v>
+        <v>100.40107154147225</v>
       </c>
       <c r="B36">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>4.0502181540662248</v>
+        <v>100.44109849962079</v>
       </c>
       <c r="B37">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>4.05477170243587</v>
+        <v>100.48112545776932</v>
       </c>
       <c r="B38">
-        <v>176</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>4.0593252508055144</v>
+        <v>100.52115241591787</v>
       </c>
       <c r="B39">
-        <v>163</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>4.0638787991751588</v>
+        <v>100.56117937406641</v>
       </c>
       <c r="B40">
-        <v>111</v>
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>4.0684323475448041</v>
+        <v>100.60120633221494</v>
       </c>
       <c r="B41">
-        <v>113</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>4.0729858959144485</v>
+        <v>100.64123329036349</v>
       </c>
       <c r="B42">
-        <v>98</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>4.0775394442840929</v>
+        <v>100.68126024851203</v>
       </c>
       <c r="B43">
-        <v>66</v>
+        <v>195</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>4.0820929926537382</v>
+        <v>100.72128720666056</v>
       </c>
       <c r="B44">
-        <v>68</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>4.0866465410233825</v>
+        <v>100.76131416480911</v>
       </c>
       <c r="B45">
-        <v>35</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>4.0912000893930269</v>
+        <v>100.80134112295765</v>
       </c>
       <c r="B46">
-        <v>30</v>
+        <v>174</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>4.0957536377626722</v>
+        <v>100.84136808110618</v>
       </c>
       <c r="B47">
-        <v>24</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>4.1003071861323166</v>
+        <v>100.88139503925473</v>
       </c>
       <c r="B48">
-        <v>22</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>4.104860734501961</v>
+        <v>100.92142199740327</v>
       </c>
       <c r="B49">
-        <v>9</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>4.1094142828716063</v>
+        <v>100.9614489555518</v>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1243,12 +2983,826 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>19800.069861439828</v>
+      </c>
+      <c r="B1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>19808.07616823824</v>
+      </c>
+      <c r="B2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>19816.082475036648</v>
+      </c>
+      <c r="B3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>19824.08878183506</v>
+      </c>
+      <c r="B4">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19832.095088633469</v>
+      </c>
+      <c r="B5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>19840.101395431881</v>
+      </c>
+      <c r="B6">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>19848.107702230289</v>
+      </c>
+      <c r="B7">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>19856.114009028701</v>
+      </c>
+      <c r="B8">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>19864.120315827109</v>
+      </c>
+      <c r="B9">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>19872.126622625521</v>
+      </c>
+      <c r="B10">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>19880.132929423929</v>
+      </c>
+      <c r="B11">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>19888.139236222341</v>
+      </c>
+      <c r="B12">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>19896.14554302075</v>
+      </c>
+      <c r="B13">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>19904.151849819162</v>
+      </c>
+      <c r="B14">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>19912.15815661757</v>
+      </c>
+      <c r="B15">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>19920.164463415982</v>
+      </c>
+      <c r="B16">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>19928.17077021439</v>
+      </c>
+      <c r="B17">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>19936.177077012802</v>
+      </c>
+      <c r="B18">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19944.183383811211</v>
+      </c>
+      <c r="B19">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19952.189690609623</v>
+      </c>
+      <c r="B20">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19960.195997408031</v>
+      </c>
+      <c r="B21">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19968.202304206443</v>
+      </c>
+      <c r="B22">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>19976.208611004851</v>
+      </c>
+      <c r="B23">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>19984.214917803263</v>
+      </c>
+      <c r="B24">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>19992.221224601672</v>
+      </c>
+      <c r="B25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>20000.227531400084</v>
+      </c>
+      <c r="B26">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>20008.233838198496</v>
+      </c>
+      <c r="B27">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>20016.240144996904</v>
+      </c>
+      <c r="B28">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>20024.246451795316</v>
+      </c>
+      <c r="B29">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>20032.252758593724</v>
+      </c>
+      <c r="B30">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>20040.259065392136</v>
+      </c>
+      <c r="B31">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>20048.265372190544</v>
+      </c>
+      <c r="B32">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>20056.271678988956</v>
+      </c>
+      <c r="B33">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>20064.277985787365</v>
+      </c>
+      <c r="B34">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>20072.284292585777</v>
+      </c>
+      <c r="B35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>20080.290599384185</v>
+      </c>
+      <c r="B36">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>20088.296906182597</v>
+      </c>
+      <c r="B37">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>20096.303212981005</v>
+      </c>
+      <c r="B38">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>20104.309519779417</v>
+      </c>
+      <c r="B39">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>20112.315826577826</v>
+      </c>
+      <c r="B40">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>20120.322133376238</v>
+      </c>
+      <c r="B41">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>20128.328440174646</v>
+      </c>
+      <c r="B42">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>20136.334746973058</v>
+      </c>
+      <c r="B43">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>20144.341053771466</v>
+      </c>
+      <c r="B44">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>20152.347360569878</v>
+      </c>
+      <c r="B45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>20160.353667368287</v>
+      </c>
+      <c r="B46">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>20168.359974166699</v>
+      </c>
+      <c r="B47">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>20176.366280965107</v>
+      </c>
+      <c r="B48">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>20184.372587763519</v>
+      </c>
+      <c r="B49">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>20192.378894561927</v>
+      </c>
+      <c r="B50">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>19.430968263251035</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>19.453834612667048</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>19.476700962083061</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>19.499567311499074</v>
+      </c>
+      <c r="B4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>19.522433660915087</v>
+      </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>19.545300010331104</v>
+      </c>
+      <c r="B6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>19.568166359747117</v>
+      </c>
+      <c r="B7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>19.59103270916313</v>
+      </c>
+      <c r="B8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>19.613899058579143</v>
+      </c>
+      <c r="B9">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>19.636765407995156</v>
+      </c>
+      <c r="B10">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>19.659631757411169</v>
+      </c>
+      <c r="B11">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>19.682498106827182</v>
+      </c>
+      <c r="B12">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>19.705364456243196</v>
+      </c>
+      <c r="B13">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>19.728230805659209</v>
+      </c>
+      <c r="B14">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>19.751097155075222</v>
+      </c>
+      <c r="B15">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>19.773963504491235</v>
+      </c>
+      <c r="B16">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>19.796829853907251</v>
+      </c>
+      <c r="B17">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>19.819696203323264</v>
+      </c>
+      <c r="B18">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>19.842562552739277</v>
+      </c>
+      <c r="B19">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19.865428902155291</v>
+      </c>
+      <c r="B20">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19.888295251571304</v>
+      </c>
+      <c r="B21">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19.911161600987317</v>
+      </c>
+      <c r="B22">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>19.93402795040333</v>
+      </c>
+      <c r="B23">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>19.956894299819343</v>
+      </c>
+      <c r="B24">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>19.979760649235356</v>
+      </c>
+      <c r="B25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>20.002626998651373</v>
+      </c>
+      <c r="B26">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>20.025493348067386</v>
+      </c>
+      <c r="B27">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>20.048359697483399</v>
+      </c>
+      <c r="B28">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>20.071226046899412</v>
+      </c>
+      <c r="B29">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>20.094092396315425</v>
+      </c>
+      <c r="B30">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>20.116958745731438</v>
+      </c>
+      <c r="B31">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>20.139825095147451</v>
+      </c>
+      <c r="B32">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>20.162691444563464</v>
+      </c>
+      <c r="B33">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>20.185557793979477</v>
+      </c>
+      <c r="B34">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>20.20842414339549</v>
+      </c>
+      <c r="B35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>20.231290492811503</v>
+      </c>
+      <c r="B36">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>20.25415684222752</v>
+      </c>
+      <c r="B37">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>20.277023191643533</v>
+      </c>
+      <c r="B38">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>20.299889541059546</v>
+      </c>
+      <c r="B39">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>20.322755890475559</v>
+      </c>
+      <c r="B40">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>20.345622239891572</v>
+      </c>
+      <c r="B41">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>20.368488589307585</v>
+      </c>
+      <c r="B42">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>20.391354938723598</v>
+      </c>
+      <c r="B43">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>20.414221288139611</v>
+      </c>
+      <c r="B44">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>20.437087637555624</v>
+      </c>
+      <c r="B45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>20.459953986971641</v>
+      </c>
+      <c r="B46">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>20.482820336387654</v>
+      </c>
+      <c r="B47">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>20.505686685803667</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>20.52855303521968</v>
+      </c>
+      <c r="B49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>20.551419384635693</v>
+      </c>
+      <c r="B50">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>